<commit_message>
Refactoring ExcelWriteUtil: catch clauses in evaluateFormula integrated.
</commit_message>
<xml_diff>
--- a/ecuacion-util-poi/src/test/resources/ExcelWriteUtilTest.xlsx
+++ b/ecuacion-util-poi/src/test/resources/ExcelWriteUtilTest.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-utils/ecuacion-util-poi/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2736DD-04AC-8E48-A5A1-BB639C13685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6438A6E-0FFA-5340-BBEE-F3D5F63D0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" activeTab="1" xr2:uid="{2468A711-9CE9-774B-B2CD-5C8D199E7A03}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16640" activeTab="1" xr2:uid="{2468A711-9CE9-774B-B2CD-5C8D199E7A03}"/>
   </bookViews>
   <sheets>
     <sheet name="getReadyToEvaluateFormulaTest" sheetId="4" r:id="rId1"/>
     <sheet name="evaluateFormulaTest" sheetId="5" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>2025/01/01</t>
   </si>
@@ -94,9 +97,6 @@
     <t>target cell</t>
   </si>
   <si>
-    <t>calculations</t>
-  </si>
-  <si>
     <t>FormulaParseException</t>
   </si>
   <si>
@@ -107,6 +107,42 @@
   </si>
   <si>
     <t>"#NAME?"</t>
+  </si>
+  <si>
+    <t>UnimpementedFunction Function</t>
+  </si>
+  <si>
+    <t>an unimplemented function</t>
+  </si>
+  <si>
+    <t>"#REF!"</t>
+  </si>
+  <si>
+    <t>WorkbookNotFoundException</t>
+  </si>
+  <si>
+    <t>Other error</t>
+  </si>
+  <si>
+    <t>ClassCastException</t>
+  </si>
+  <si>
+    <t>あ</t>
+  </si>
+  <si>
+    <t>"#VALUE!"</t>
+  </si>
+  <si>
+    <t>(No Exception)</t>
+  </si>
+  <si>
+    <t>"#DIV/0!"</t>
+  </si>
+  <si>
+    <t>"#N/A"</t>
+  </si>
+  <si>
+    <t>values for calculation</t>
   </si>
 </sst>
 </file>
@@ -217,7 +253,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -230,10 +266,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -244,9 +280,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -267,6 +300,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Summary"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,13 +735,13 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -704,81 +750,132 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>13</v>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="str" cm="1">
+        <f t="array" ref="B4">_xlfn.TEXTSPLIT(D4,",")</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="e" cm="1">
-        <f t="array" ref="B4">vlooku</f>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="e" cm="1">
+        <f t="array" ref="B5">vlooku</f>
         <v>#NAME?</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="e">
+        <f>[1]Summary!$A$1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="e">
+        <f>D7/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="e">
+        <f>1/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="e">
+        <f>VLOOKUP("abc",H3:I6,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="e" cm="1">
+        <f t="array" ref="B10">_xlfn.IFS(D10,"A",TRUE,"B")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="e">
+        <f>VLOOKUP("abc",H3:I6,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>

</xml_diff>